<commit_message>
Early GUI and Rollup classes
GUI in SWING
'Business' class that serves to rollup Organizations and Buildings with
Owners and Managers - Need to finalize this class and integrate with the
settlement rollup logic.
</commit_message>
<xml_diff>
--- a/RoomsExcelSpreadsheet.xlsx
+++ b/RoomsExcelSpreadsheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="14370" firstSheet="1" activeTab="6"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="20730" windowHeight="11760" firstSheet="2" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="RoomsExcelSpreadsheet" sheetId="1" r:id="rId1"/>
@@ -14,6 +14,7 @@
     <sheet name="Qualities" sheetId="5" r:id="rId5"/>
     <sheet name="Managers" sheetId="6" r:id="rId6"/>
     <sheet name="Teams" sheetId="7" r:id="rId7"/>
+    <sheet name="OrganizationsCSV" sheetId="8" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="roomCSV" localSheetId="2">Augmentation!$A$2:$I$2</definedName>
@@ -75,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1810" uniqueCount="902">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1864" uniqueCount="954">
   <si>
     <t>Name</t>
   </si>
@@ -3002,12 +3003,168 @@
   <si>
     <t>Soldiers are trained in combat and have the means and will to kill your enemies. Unlike Guards, Soldiers actively engage in fighting on behest of a leader (although you can make Soldiers act as Guards). Depending on the nature of your organization, they might be enforcers rather than military-style soldiers. They are typically 1st-level warriors, each with scale mail, a longsword, a heavy wooden shield, and javelins.</t>
   </si>
+  <si>
+    <t>Teams</t>
+  </si>
+  <si>
+    <t>Artisans' Guild</t>
+  </si>
+  <si>
+    <t>Artisans and assistants who create quality goods.</t>
+  </si>
+  <si>
+    <t>1 Bureaucrat,2 Craftspeople,2 Laborers</t>
+  </si>
+  <si>
+    <t>Bounty Hunters</t>
+  </si>
+  <si>
+    <t>1 Archers,1 Bureaucrats,1 Driver</t>
+  </si>
+  <si>
+    <t>Fighters trained to find and capture criminals and escapees.</t>
+  </si>
+  <si>
+    <t>Brute Squad</t>
+  </si>
+  <si>
+    <t>A gang of well-armed professionals who throw their weight around on your behalf.</t>
+  </si>
+  <si>
+    <t>1 Robbers,2 Soldiers</t>
+  </si>
+  <si>
+    <t>Cabal</t>
+  </si>
+  <si>
+    <t>A study group of peers and apprentices devoted to arcane mysteries and research</t>
+  </si>
+  <si>
+    <t>4 Apprentice,1 Mage,1 Sage</t>
+  </si>
+  <si>
+    <t>Caravan Crew</t>
+  </si>
+  <si>
+    <t>Travelers skilled in loading, transporting and unloading trade goods from animals, wagons and ships</t>
+  </si>
+  <si>
+    <t>2 Driver,1 Guards,1 Laborers</t>
+  </si>
+  <si>
+    <t>Cult</t>
+  </si>
+  <si>
+    <t>A splinter religion or secret society that believes yours is the true faith</t>
+  </si>
+  <si>
+    <t>4 Acolyte,2 Guards,1 Priest</t>
+  </si>
+  <si>
+    <t>Entourage</t>
+  </si>
+  <si>
+    <t>Friends and toadies who take care of your eating, sleeping, travel and entertainment arrangements</t>
+  </si>
+  <si>
+    <t>1 Bureaucrat,1 Driver,2 Lackeys</t>
+  </si>
+  <si>
+    <t>Fight Club</t>
+  </si>
+  <si>
+    <t>A possibly illegal association of boxing adicionados</t>
+  </si>
+  <si>
+    <t>1 Driver,1 Guards,1 Laborers,1 Lackeys,1 Scofflaws</t>
+  </si>
+  <si>
+    <t>Hunting Party</t>
+  </si>
+  <si>
+    <t>The necessary guides and assistants for sport hunting</t>
+  </si>
+  <si>
+    <t>1 Archers,1 Laborers,1 Lackeys</t>
+  </si>
+  <si>
+    <t>Mercenary Company</t>
+  </si>
+  <si>
+    <t>A well-armed group of warriors who are loyal to you, and who are paid to guard or fight</t>
+  </si>
+  <si>
+    <t>1 Elite Archers,2 Elite Soldiers,1 Priest</t>
+  </si>
+  <si>
+    <t>Ship Crew</t>
+  </si>
+  <si>
+    <t>The crew of a small sailing vessel</t>
+  </si>
+  <si>
+    <t>1 Laborers,1 Sailors</t>
+  </si>
+  <si>
+    <t>Theater Company</t>
+  </si>
+  <si>
+    <t>Performers, Set Dressers and Costumers for an acting troupe or similar group</t>
+  </si>
+  <si>
+    <t>5 Apprentice,1 Bureaucrat,1 Craftspeople,1 Laborers</t>
+  </si>
+  <si>
+    <t>Medical Team</t>
+  </si>
+  <si>
+    <t>A skilled team of healers and their assistants</t>
+  </si>
+  <si>
+    <t>1 Bureaucrat,2 Priest,1 Sage</t>
+  </si>
+  <si>
+    <t>A skilled team of researchers to provide advice on a variety of subjects</t>
+  </si>
+  <si>
+    <t>2 Apprentice, 3 Sage, 1 Mage, 1 Priest</t>
+  </si>
+  <si>
+    <t>Thieves Guild</t>
+  </si>
+  <si>
+    <t>A band of criminals and thugs who commit illegal acts</t>
+  </si>
+  <si>
+    <t>2 Cutpurses,1 Robbers,1 Scofflaws,1 Soldiers</t>
+  </si>
+  <si>
+    <t>Vagabonds</t>
+  </si>
+  <si>
+    <t>Unsavory wanderers skilled at stage magic, fortunetelling, rigged games and snake oil.</t>
+  </si>
+  <si>
+    <t>1 Acolyte,1 Apprentice,1 Cutpurse,2 Driver,1 Guards,1 Laborers,1 Scofflaws</t>
+  </si>
+  <si>
+    <t>Archivists</t>
+  </si>
+  <si>
+    <t>Farmhands</t>
+  </si>
+  <si>
+    <t>A team of farmhands to handle any agricultural need.</t>
+  </si>
+  <si>
+    <t>2 Driver,4 Laborers</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3045,6 +3202,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -3067,11 +3231,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -8384,15 +8551,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC79"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AB38" sqref="AB38"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="3" width="15.28515625" customWidth="1"/>
-    <col min="4" max="20" width="9.140625" hidden="1" customWidth="1"/>
-    <col min="21" max="21" width="9.140625" customWidth="1"/>
+    <col min="4" max="21" width="9.140625" customWidth="1"/>
     <col min="22" max="22" width="11.85546875" customWidth="1"/>
     <col min="23" max="23" width="12.85546875" customWidth="1"/>
     <col min="24" max="26" width="9.140625" customWidth="1"/>
@@ -20136,7 +20302,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20408,8 +20574,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S14" sqref="S14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="S20" sqref="S20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21775,4 +21941,223 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.85546875" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" t="s">
+        <v>902</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>950</v>
+      </c>
+      <c r="B2" t="s">
+        <v>942</v>
+      </c>
+      <c r="C2" t="s">
+        <v>943</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>903</v>
+      </c>
+      <c r="B3" t="s">
+        <v>904</v>
+      </c>
+      <c r="C3" t="s">
+        <v>905</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>906</v>
+      </c>
+      <c r="B4" t="s">
+        <v>908</v>
+      </c>
+      <c r="C4" t="s">
+        <v>907</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>909</v>
+      </c>
+      <c r="B5" t="s">
+        <v>910</v>
+      </c>
+      <c r="C5" t="s">
+        <v>911</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>912</v>
+      </c>
+      <c r="B6" t="s">
+        <v>913</v>
+      </c>
+      <c r="C6" t="s">
+        <v>914</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>915</v>
+      </c>
+      <c r="B7" t="s">
+        <v>916</v>
+      </c>
+      <c r="C7" t="s">
+        <v>917</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>918</v>
+      </c>
+      <c r="B8" t="s">
+        <v>919</v>
+      </c>
+      <c r="C8" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>921</v>
+      </c>
+      <c r="B9" t="s">
+        <v>922</v>
+      </c>
+      <c r="C9" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>951</v>
+      </c>
+      <c r="B10" t="s">
+        <v>952</v>
+      </c>
+      <c r="C10" t="s">
+        <v>953</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>924</v>
+      </c>
+      <c r="B11" t="s">
+        <v>925</v>
+      </c>
+      <c r="C11" t="s">
+        <v>926</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>927</v>
+      </c>
+      <c r="B12" t="s">
+        <v>928</v>
+      </c>
+      <c r="C12" t="s">
+        <v>929</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>939</v>
+      </c>
+      <c r="B13" t="s">
+        <v>940</v>
+      </c>
+      <c r="C13" t="s">
+        <v>941</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>930</v>
+      </c>
+      <c r="B14" t="s">
+        <v>931</v>
+      </c>
+      <c r="C14" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>933</v>
+      </c>
+      <c r="B15" t="s">
+        <v>934</v>
+      </c>
+      <c r="C15" t="s">
+        <v>935</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>936</v>
+      </c>
+      <c r="B16" t="s">
+        <v>937</v>
+      </c>
+      <c r="C16" t="s">
+        <v>938</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>944</v>
+      </c>
+      <c r="B17" t="s">
+        <v>945</v>
+      </c>
+      <c r="C17" t="s">
+        <v>946</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>947</v>
+      </c>
+      <c r="B18" t="s">
+        <v>948</v>
+      </c>
+      <c r="C18" t="s">
+        <v>949</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="5" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>